<commit_message>
Atualizado por script em 30-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/colombia_primera-a_2023.xlsx
+++ b/2023/colombia_primera-a_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V213"/>
+  <dimension ref="A1:V215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18697,22 +18697,22 @@
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>America De Cali</t>
+          <t>Atl. Nacional</t>
         </is>
       </c>
       <c r="G199" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>Bucaramanga</t>
+          <t>Deportes Tolima</t>
         </is>
       </c>
       <c r="I199" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J199" t="n">
-        <v>1.46</v>
+        <v>1.99</v>
       </c>
       <c r="K199" t="inlineStr">
         <is>
@@ -18720,7 +18720,7 @@
         </is>
       </c>
       <c r="L199" t="n">
-        <v>1.4</v>
+        <v>1.87</v>
       </c>
       <c r="M199" t="inlineStr">
         <is>
@@ -18728,7 +18728,7 @@
         </is>
       </c>
       <c r="N199" t="n">
-        <v>4.38</v>
+        <v>3.32</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -18736,15 +18736,15 @@
         </is>
       </c>
       <c r="P199" t="n">
-        <v>4.66</v>
+        <v>3.44</v>
       </c>
       <c r="Q199" t="inlineStr">
         <is>
-          <t>09/11/2023 01:29</t>
+          <t>09/11/2023 01:23</t>
         </is>
       </c>
       <c r="R199" t="n">
-        <v>7.32</v>
+        <v>4.17</v>
       </c>
       <c r="S199" t="inlineStr">
         <is>
@@ -18752,16 +18752,16 @@
         </is>
       </c>
       <c r="T199" t="n">
-        <v>8.09</v>
+        <v>4.53</v>
       </c>
       <c r="U199" t="inlineStr">
         <is>
-          <t>09/11/2023 01:29</t>
+          <t>09/11/2023 01:26</t>
         </is>
       </c>
       <c r="V199" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-a/america-de-cali-bucaramanga/IVL60qj5/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-a/atl-nacional-deportes-tolima/MNINd1kU/</t>
         </is>
       </c>
     </row>
@@ -18789,22 +18789,22 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>Atl. Nacional</t>
+          <t>America De Cali</t>
         </is>
       </c>
       <c r="G200" t="n">
+        <v>1</v>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="I200" t="n">
         <v>2</v>
       </c>
-      <c r="H200" t="inlineStr">
-        <is>
-          <t>Deportes Tolima</t>
-        </is>
-      </c>
-      <c r="I200" t="n">
-        <v>3</v>
-      </c>
       <c r="J200" t="n">
-        <v>1.99</v>
+        <v>1.46</v>
       </c>
       <c r="K200" t="inlineStr">
         <is>
@@ -18812,7 +18812,7 @@
         </is>
       </c>
       <c r="L200" t="n">
-        <v>1.87</v>
+        <v>1.4</v>
       </c>
       <c r="M200" t="inlineStr">
         <is>
@@ -18820,7 +18820,7 @@
         </is>
       </c>
       <c r="N200" t="n">
-        <v>3.32</v>
+        <v>4.38</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -18828,15 +18828,15 @@
         </is>
       </c>
       <c r="P200" t="n">
-        <v>3.44</v>
+        <v>4.66</v>
       </c>
       <c r="Q200" t="inlineStr">
         <is>
-          <t>09/11/2023 01:23</t>
+          <t>09/11/2023 01:29</t>
         </is>
       </c>
       <c r="R200" t="n">
-        <v>4.17</v>
+        <v>7.32</v>
       </c>
       <c r="S200" t="inlineStr">
         <is>
@@ -18844,16 +18844,16 @@
         </is>
       </c>
       <c r="T200" t="n">
-        <v>4.53</v>
+        <v>8.09</v>
       </c>
       <c r="U200" t="inlineStr">
         <is>
-          <t>09/11/2023 01:26</t>
+          <t>09/11/2023 01:29</t>
         </is>
       </c>
       <c r="V200" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-a/atl-nacional-deportes-tolima/MNINd1kU/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-a/america-de-cali-bucaramanga/IVL60qj5/</t>
         </is>
       </c>
     </row>
@@ -20050,6 +20050,190 @@
       <c r="V213" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/colombia/primera-a/atl-nacional-america-de-cali/EgwRXggB/</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>primera-a</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E214" s="2" t="n">
+        <v>45260.01041666666</v>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>Aguilas</t>
+        </is>
+      </c>
+      <c r="G214" t="n">
+        <v>1</v>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>Junior</t>
+        </is>
+      </c>
+      <c r="I214" t="n">
+        <v>1</v>
+      </c>
+      <c r="J214" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="K214" t="inlineStr">
+        <is>
+          <t>26/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="L214" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="M214" t="inlineStr">
+        <is>
+          <t>30/11/2023 00:11</t>
+        </is>
+      </c>
+      <c r="N214" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="O214" t="inlineStr">
+        <is>
+          <t>26/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="P214" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="Q214" t="inlineStr">
+        <is>
+          <t>30/11/2023 00:11</t>
+        </is>
+      </c>
+      <c r="R214" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="S214" t="inlineStr">
+        <is>
+          <t>26/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="T214" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="U214" t="inlineStr">
+        <is>
+          <t>30/11/2023 00:11</t>
+        </is>
+      </c>
+      <c r="V214" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-a/aguilas-doradas-junior/tEEOkEab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>primera-a</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E215" s="2" t="n">
+        <v>45260.10416666666</v>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>Dep. Cali</t>
+        </is>
+      </c>
+      <c r="G215" t="n">
+        <v>0</v>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>Deportes Tolima</t>
+        </is>
+      </c>
+      <c r="I215" t="n">
+        <v>2</v>
+      </c>
+      <c r="J215" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="K215" t="inlineStr">
+        <is>
+          <t>25/11/2023 23:12</t>
+        </is>
+      </c>
+      <c r="L215" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="M215" t="inlineStr">
+        <is>
+          <t>30/11/2023 02:26</t>
+        </is>
+      </c>
+      <c r="N215" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="O215" t="inlineStr">
+        <is>
+          <t>25/11/2023 23:12</t>
+        </is>
+      </c>
+      <c r="P215" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="Q215" t="inlineStr">
+        <is>
+          <t>30/11/2023 02:21</t>
+        </is>
+      </c>
+      <c r="R215" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="S215" t="inlineStr">
+        <is>
+          <t>25/11/2023 23:12</t>
+        </is>
+      </c>
+      <c r="T215" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="U215" t="inlineStr">
+        <is>
+          <t>30/11/2023 02:26</t>
+        </is>
+      </c>
+      <c r="V215" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-a/dep-cali-deportes-tolima/K4DSlYE4/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 01-12-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/colombia_primera-a_2023.xlsx
+++ b/2023/colombia_primera-a_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V215"/>
+  <dimension ref="A1:V217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18605,22 +18605,22 @@
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t>La Equidad</t>
+          <t>Jaguares de Cordoba</t>
         </is>
       </c>
       <c r="G198" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>Millonarios</t>
+          <t>Aguilas</t>
         </is>
       </c>
       <c r="I198" t="n">
         <v>1</v>
       </c>
       <c r="J198" t="n">
-        <v>2.39</v>
+        <v>3.28</v>
       </c>
       <c r="K198" t="inlineStr">
         <is>
@@ -18628,15 +18628,15 @@
         </is>
       </c>
       <c r="L198" t="n">
-        <v>2.11</v>
+        <v>3.85</v>
       </c>
       <c r="M198" t="inlineStr">
         <is>
-          <t>09/11/2023 01:26</t>
+          <t>09/11/2023 01:29</t>
         </is>
       </c>
       <c r="N198" t="n">
-        <v>2.94</v>
+        <v>2.99</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -18644,15 +18644,15 @@
         </is>
       </c>
       <c r="P198" t="n">
-        <v>3.02</v>
+        <v>2.99</v>
       </c>
       <c r="Q198" t="inlineStr">
         <is>
-          <t>09/11/2023 01:26</t>
+          <t>09/11/2023 01:28</t>
         </is>
       </c>
       <c r="R198" t="n">
-        <v>3.52</v>
+        <v>2.48</v>
       </c>
       <c r="S198" t="inlineStr">
         <is>
@@ -18660,16 +18660,16 @@
         </is>
       </c>
       <c r="T198" t="n">
-        <v>4.16</v>
+        <v>2.22</v>
       </c>
       <c r="U198" t="inlineStr">
         <is>
-          <t>09/11/2023 01:26</t>
+          <t>09/11/2023 01:29</t>
         </is>
       </c>
       <c r="V198" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-a/la-equidad-millonarios/vuN21Pza/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-a/jaguares-de-cordoba-aguilas-doradas/dGXc25Lh/</t>
         </is>
       </c>
     </row>
@@ -18697,7 +18697,7 @@
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>Atl. Nacional</t>
+          <t>La Equidad</t>
         </is>
       </c>
       <c r="G199" t="n">
@@ -18705,14 +18705,14 @@
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>Deportes Tolima</t>
+          <t>Millonarios</t>
         </is>
       </c>
       <c r="I199" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J199" t="n">
-        <v>1.99</v>
+        <v>2.39</v>
       </c>
       <c r="K199" t="inlineStr">
         <is>
@@ -18720,7 +18720,7 @@
         </is>
       </c>
       <c r="L199" t="n">
-        <v>1.87</v>
+        <v>2.11</v>
       </c>
       <c r="M199" t="inlineStr">
         <is>
@@ -18728,7 +18728,7 @@
         </is>
       </c>
       <c r="N199" t="n">
-        <v>3.32</v>
+        <v>2.94</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -18736,15 +18736,15 @@
         </is>
       </c>
       <c r="P199" t="n">
-        <v>3.44</v>
+        <v>3.02</v>
       </c>
       <c r="Q199" t="inlineStr">
         <is>
-          <t>09/11/2023 01:23</t>
+          <t>09/11/2023 01:26</t>
         </is>
       </c>
       <c r="R199" t="n">
-        <v>4.17</v>
+        <v>3.52</v>
       </c>
       <c r="S199" t="inlineStr">
         <is>
@@ -18752,7 +18752,7 @@
         </is>
       </c>
       <c r="T199" t="n">
-        <v>4.53</v>
+        <v>4.16</v>
       </c>
       <c r="U199" t="inlineStr">
         <is>
@@ -18761,7 +18761,7 @@
       </c>
       <c r="V199" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-a/atl-nacional-deportes-tolima/MNINd1kU/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-a/la-equidad-millonarios/vuN21Pza/</t>
         </is>
       </c>
     </row>
@@ -18881,22 +18881,22 @@
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>Jaguares de Cordoba</t>
+          <t>Atl. Nacional</t>
         </is>
       </c>
       <c r="G201" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>Aguilas</t>
+          <t>Deportes Tolima</t>
         </is>
       </c>
       <c r="I201" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J201" t="n">
-        <v>3.28</v>
+        <v>1.99</v>
       </c>
       <c r="K201" t="inlineStr">
         <is>
@@ -18904,15 +18904,15 @@
         </is>
       </c>
       <c r="L201" t="n">
-        <v>3.85</v>
+        <v>1.87</v>
       </c>
       <c r="M201" t="inlineStr">
         <is>
-          <t>09/11/2023 01:29</t>
+          <t>09/11/2023 01:26</t>
         </is>
       </c>
       <c r="N201" t="n">
-        <v>2.99</v>
+        <v>3.32</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -18920,15 +18920,15 @@
         </is>
       </c>
       <c r="P201" t="n">
-        <v>2.99</v>
+        <v>3.44</v>
       </c>
       <c r="Q201" t="inlineStr">
         <is>
-          <t>09/11/2023 01:28</t>
+          <t>09/11/2023 01:23</t>
         </is>
       </c>
       <c r="R201" t="n">
-        <v>2.48</v>
+        <v>4.17</v>
       </c>
       <c r="S201" t="inlineStr">
         <is>
@@ -18936,16 +18936,16 @@
         </is>
       </c>
       <c r="T201" t="n">
-        <v>2.22</v>
+        <v>4.53</v>
       </c>
       <c r="U201" t="inlineStr">
         <is>
-          <t>09/11/2023 01:29</t>
+          <t>09/11/2023 01:26</t>
         </is>
       </c>
       <c r="V201" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-a/jaguares-de-cordoba-aguilas-doradas/dGXc25Lh/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-a/atl-nacional-deportes-tolima/MNINd1kU/</t>
         </is>
       </c>
     </row>
@@ -20234,6 +20234,190 @@
       <c r="V215" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/colombia/primera-a/dep-cali-deportes-tolima/K4DSlYE4/</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>primera-a</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E216" s="2" t="n">
+        <v>45261.01041666666</v>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>America De Cali</t>
+        </is>
+      </c>
+      <c r="G216" t="n">
+        <v>0</v>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>Atl. Nacional</t>
+        </is>
+      </c>
+      <c r="I216" t="n">
+        <v>1</v>
+      </c>
+      <c r="J216" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="K216" t="inlineStr">
+        <is>
+          <t>27/11/2023 00:42</t>
+        </is>
+      </c>
+      <c r="L216" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="M216" t="inlineStr">
+        <is>
+          <t>01/12/2023 00:13</t>
+        </is>
+      </c>
+      <c r="N216" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="O216" t="inlineStr">
+        <is>
+          <t>27/11/2023 00:42</t>
+        </is>
+      </c>
+      <c r="P216" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="Q216" t="inlineStr">
+        <is>
+          <t>01/12/2023 00:14</t>
+        </is>
+      </c>
+      <c r="R216" t="n">
+        <v>5.16</v>
+      </c>
+      <c r="S216" t="inlineStr">
+        <is>
+          <t>27/11/2023 00:42</t>
+        </is>
+      </c>
+      <c r="T216" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="U216" t="inlineStr">
+        <is>
+          <t>01/12/2023 00:14</t>
+        </is>
+      </c>
+      <c r="V216" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-a/america-de-cali-atl-nacional/ERCWmhUA/</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>primera-a</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E217" s="2" t="n">
+        <v>45261.10416666666</v>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>Ind. Medellin</t>
+        </is>
+      </c>
+      <c r="G217" t="n">
+        <v>2</v>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>Millonarios</t>
+        </is>
+      </c>
+      <c r="I217" t="n">
+        <v>1</v>
+      </c>
+      <c r="J217" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="K217" t="inlineStr">
+        <is>
+          <t>26/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="L217" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="M217" t="inlineStr">
+        <is>
+          <t>01/12/2023 02:28</t>
+        </is>
+      </c>
+      <c r="N217" t="n">
+        <v>3.31</v>
+      </c>
+      <c r="O217" t="inlineStr">
+        <is>
+          <t>26/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P217" t="n">
+        <v>2.97</v>
+      </c>
+      <c r="Q217" t="inlineStr">
+        <is>
+          <t>01/12/2023 02:22</t>
+        </is>
+      </c>
+      <c r="R217" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="S217" t="inlineStr">
+        <is>
+          <t>26/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="T217" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="U217" t="inlineStr">
+        <is>
+          <t>01/12/2023 02:28</t>
+        </is>
+      </c>
+      <c r="V217" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-a/ind-medellin-millonarios/Q1GzmCqH/</t>
         </is>
       </c>
     </row>

</xml_diff>